<commit_message>
first run of including pattern in csv
</commit_message>
<xml_diff>
--- a/test/PDFLib/PDFLib_SampleSizes_Excel.xlsx
+++ b/test/PDFLib/PDFLib_SampleSizes_Excel.xlsx
@@ -19751,15 +19751,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>0</xdr:col>
-      <xdr:colOff>9525</xdr:colOff>
+      <xdr:colOff>0</xdr:colOff>
       <xdr:row>2</xdr:row>
-      <xdr:rowOff>142875</xdr:rowOff>
+      <xdr:rowOff>85725</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>13</xdr:col>
-      <xdr:colOff>466724</xdr:colOff>
+      <xdr:colOff>457199</xdr:colOff>
       <xdr:row>23</xdr:row>
-      <xdr:rowOff>171450</xdr:rowOff>
+      <xdr:rowOff>114300</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -20091,7 +20091,7 @@
   <dimension ref="A1:H2172"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G2" sqref="G2"/>
+      <selection activeCell="F1" sqref="F1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -20101,7 +20101,7 @@
     <col min="3" max="3" width="8.5703125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="7.42578125" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="7" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="37.7109375" customWidth="1"/>
+    <col min="6" max="6" width="43.28515625" customWidth="1"/>
     <col min="7" max="7" width="15.42578125" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="15.7109375" bestFit="1" customWidth="1"/>
   </cols>

</xml_diff>